<commit_message>
Version 1.3.0  | Open AAI Control Room Complet| Re Framework Configurations complete | Structure In Progress|
</commit_message>
<xml_diff>
--- a/Data/Input/input.xlsx
+++ b/Data/Input/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josea.macias\Documents\UiPath\ScheduleBot Runners UnAttended AAI 360\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2011C160-0727-4727-B2BB-F1A0AACEE42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD66ECE-FBCE-44C9-948A-9DCC47CA3A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,9 +138,6 @@
     <t>https://community.cloud.automationanywhere.digital/#/login?</t>
   </si>
   <si>
-    <t>jose.maciast@ecci.edu.co</t>
-  </si>
-  <si>
     <t>Japon202!@</t>
   </si>
   <si>
@@ -153,28 +150,31 @@
     <t>Password_ControlRoom</t>
   </si>
   <si>
-    <t>Transacción N 816e9b2f-453f-42c3-83f6-74398a4e842e</t>
-  </si>
-  <si>
-    <t>Transacción N fbb37cc6-4f99-41ce-b153-6d5209fe4d5c</t>
-  </si>
-  <si>
-    <t>Transacción N 53dad985-5773-466f-ade0-3b7fb7a50140</t>
-  </si>
-  <si>
-    <t>Transacción N 10959fce-1dc1-4254-be5f-7269730283ca</t>
-  </si>
-  <si>
-    <t>Transacción N 4e72f981-aff2-4632-bb0d-7ce4c32a3051</t>
-  </si>
-  <si>
-    <t>Transacción N 879803b4-ce65-406e-b2ce-7a4751abace0</t>
-  </si>
-  <si>
     <t>Transacción N 4c1e64c4-b543-4dfe-bf48-5677b6f78f49</t>
   </si>
   <si>
     <t>Transacción N 94b1961d-bc2b-4527-b29f-d104e19e7fa3</t>
+  </si>
+  <si>
+    <t>josea.maciast@ecci.edu.co</t>
+  </si>
+  <si>
+    <t>Transacción N a915ff59-eb8f-4817-946e-2cb5da370461</t>
+  </si>
+  <si>
+    <t>Transacción N 1a0ad5f1-0397-4eb0-a8dc-768c9e2ce2a8</t>
+  </si>
+  <si>
+    <t>Transacción N fbffd5fe-cc28-42ac-ab1b-f794eea3475e</t>
+  </si>
+  <si>
+    <t>Transacción N fb51aedc-fe4f-4004-aa7b-f2352526267f</t>
+  </si>
+  <si>
+    <t>Transacción N 33d18ab6-3442-4fe4-ad3a-5f2e129bf3e6</t>
+  </si>
+  <si>
+    <t>Transacción N 6fdfed77-67a9-4b74-878e-44ed268fc753</t>
   </si>
 </sst>
 </file>
@@ -585,7 +585,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I10" sqref="F2:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,18 +607,18 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>36</v>
-      </c>
-      <c r="G1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -633,15 +633,15 @@
         <v>32</v>
       </c>
       <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
         <v>33</v>
-      </c>
-      <c r="G2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -656,15 +656,15 @@
         <v>32</v>
       </c>
       <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
         <v>33</v>
-      </c>
-      <c r="G3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -679,15 +679,15 @@
         <v>32</v>
       </c>
       <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
         <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -702,15 +702,15 @@
         <v>32</v>
       </c>
       <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
         <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -725,15 +725,15 @@
         <v>32</v>
       </c>
       <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
         <v>33</v>
-      </c>
-      <c r="G6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -748,22 +748,22 @@
         <v>32</v>
       </c>
       <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
         <v>33</v>
-      </c>
-      <c r="G7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>

</xml_diff>